<commit_message>
Artifacts for news (s3) and eventsSearch (s2) Add Filtering for date and location in events
</commit_message>
<xml_diff>
--- a/Documents/Requirements Stack Project 3 .xlsx
+++ b/Documents/Requirements Stack Project 3 .xlsx
@@ -667,9 +667,7 @@
       <c r="D14" s="1">
         <v>5.0</v>
       </c>
-      <c r="E14" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
@@ -685,9 +683,7 @@
       <c r="D15" s="1">
         <v>6.0</v>
       </c>
-      <c r="E15" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16">
@@ -703,9 +699,7 @@
       <c r="D16" s="1">
         <v>7.0</v>
       </c>
-      <c r="E16" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17">
@@ -721,9 +715,7 @@
       <c r="D17" s="1">
         <v>5.0</v>
       </c>
-      <c r="E17" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18">
@@ -739,9 +731,7 @@
       <c r="D18" s="1">
         <v>6.0</v>
       </c>
-      <c r="E18" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19">
@@ -757,9 +747,7 @@
       <c r="D19" s="1">
         <v>7.0</v>
       </c>
-      <c r="E19" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20">
@@ -775,9 +763,7 @@
       <c r="D20" s="1">
         <v>5.0</v>
       </c>
-      <c r="E20" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21">
@@ -793,9 +779,7 @@
       <c r="D21" s="1">
         <v>9.0</v>
       </c>
-      <c r="E21" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22">
@@ -811,9 +795,7 @@
       <c r="D22" s="1">
         <v>10.0</v>
       </c>
-      <c r="E22" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23">
@@ -829,9 +811,7 @@
       <c r="D23" s="1">
         <v>9.0</v>
       </c>
-      <c r="E23" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24">
@@ -847,9 +827,7 @@
       <c r="D24" s="1">
         <v>10.0</v>
       </c>
-      <c r="E24" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25">

</xml_diff>